<commit_message>
Implement navigation and state management for upload, naming, and dataset expansion flow
</commit_message>
<xml_diff>
--- a/uploads/gadget_qa_dataset_hebrew.xlsx
+++ b/uploads/gadget_qa_dataset_hebrew.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yoav/מסמכים/טכנולוגיות למידה- HIT/שנה ג/סמסטר א/פרוייקט גמר/עזרים לפרוייקט/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guesty/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4A4DD87-550E-3F4E-9C79-C9FD685F3FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA90FB1-BAD6-D04C-9203-B036F641CBD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="500" windowWidth="33540" windowHeight="18600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="33540" windowHeight="18600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>